<commit_message>
moved active elements to functions
</commit_message>
<xml_diff>
--- a/instruction_set.xlsx
+++ b/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigne\OneDrive\Desktop\projects\dsm-processor-sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAAA21-6E9B-438B-BAF5-D9FBBE4255C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC22BFE-9FFB-4E5A-BF0E-F2E8A8FB4EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{46D14E4C-D724-4611-9C4B-F0C807E422CD}"/>
   </bookViews>
@@ -1097,9 +1097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533AE942-BBBA-47B8-8C8B-6064F9B8F113}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>24</v>
@@ -1276,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>24</v>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>24</v>
@@ -1400,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>24</v>
@@ -1462,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>24</v>
@@ -1524,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>24</v>
@@ -1791,48 +1791,48 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="12">
-        <v>3</v>
-      </c>
-      <c r="E33" s="12" t="s">
+      <c r="D33" s="13">
+        <v>3</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="12">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21">
         <v>4</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="21" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2310,19 +2310,19 @@
       <c r="C56" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D56" s="9">
-        <v>3</v>
-      </c>
-      <c r="E56" s="9" t="s">
+      <c r="D56" s="26">
+        <v>3</v>
+      </c>
+      <c r="E56" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="26" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>